<commit_message>
[experiment] format results of resource constraints on NSFNET
</commit_message>
<xml_diff>
--- a/experiments/results/NSFNET/resource_constraints/summary.xlsx
+++ b/experiments/results/NSFNET/resource_constraints/summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yansen XU\Documents\Research\Projects\sfc-system\experiments\results\NSFNET\resource_constraints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F2AC41A3-BC67-4243-9543-DCD19B3C251B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B015055E-E344-4569-B0C3-145E225786F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acceptance_rate" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -491,7 +491,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -534,11 +534,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -578,6 +580,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -610,6 +613,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NSFNET-Number of VNFs=2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -711,7 +739,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$B$3:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.94799999999999995</c:v>
@@ -804,7 +832,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$C$3:$C$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.77400000000000002</c:v>
@@ -897,7 +925,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$D$3:$D$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.86199999999999999</c:v>
@@ -990,7 +1018,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$E$3:$E$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.84699999999999998</c:v>
@@ -1083,7 +1111,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$F$3:$F$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.86899999999999999</c:v>
@@ -1176,7 +1204,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$G$3:$G$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.76</c:v>
@@ -1223,6 +1251,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of SFCs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1288,7 +1371,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Acceptance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> rate</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1332,7 +1475,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3854,6 +3997,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NSFNET-Number of VNFs=3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3955,7 +4123,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$B$10:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.63</c:v>
@@ -4048,7 +4216,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$C$10:$C$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.495</c:v>
@@ -4141,7 +4309,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$D$10:$D$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.56399999999999995</c:v>
@@ -4234,7 +4402,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$E$10:$E$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.59499999999999997</c:v>
@@ -4327,7 +4495,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$F$10:$F$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.59599999999999997</c:v>
@@ -4420,7 +4588,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$G$10:$G$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.55400000000000005</c:v>
@@ -4467,6 +4635,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of SFCs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4532,7 +4755,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Acceptance rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4576,7 +4854,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4665,6 +4943,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NSFNET-Number of VNFs=4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4766,7 +5069,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$B$17:$B$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.46</c:v>
@@ -4859,7 +5162,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$C$17:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.36799999999999999</c:v>
@@ -4952,7 +5255,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$D$17:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.40500000000000003</c:v>
@@ -5045,7 +5348,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$E$17:$E$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.42799999999999999</c:v>
@@ -5138,7 +5441,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$F$17:$F$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.42499999999999999</c:v>
@@ -5231,7 +5534,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$G$17:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.39500000000000002</c:v>
@@ -5278,6 +5581,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of SFCs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5343,7 +5701,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Acceptance rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5387,7 +5800,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5476,6 +5889,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NSFNET-Number of VNFs=5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5577,7 +6015,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$B$24:$B$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.36499999999999999</c:v>
@@ -5670,7 +6108,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$C$24:$C$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.28499999999999998</c:v>
@@ -5763,7 +6201,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$D$24:$D$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.29599999999999999</c:v>
@@ -5856,7 +6294,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$E$24:$E$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.33100000000000002</c:v>
@@ -5949,7 +6387,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$F$24:$F$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.32600000000000001</c:v>
@@ -6042,7 +6480,7 @@
             <c:numRef>
               <c:f>acceptance_rate!$G$24:$G$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.32400000000000001</c:v>
@@ -6089,6 +6527,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of SFCs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6154,7 +6647,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Acceptance rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6198,7 +6746,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -17586,11 +18134,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:G28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17624,22 +18172,22 @@
       <c r="A3">
         <v>100</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0.94799999999999995</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.77400000000000002</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.86199999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.84699999999999998</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.86899999999999999</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>0.76</v>
       </c>
     </row>
@@ -17647,22 +18195,22 @@
       <c r="A4">
         <v>200</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0.46750000000000003</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0.40250000000000002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>0.45450000000000002</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0.45250000000000001</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>0.44550000000000001</v>
       </c>
     </row>
@@ -17670,22 +18218,22 @@
       <c r="A5">
         <v>300</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.321666666667</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.262666666667</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>0.307</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.306333333333</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>0.30499999999999999</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>0.29233333333299999</v>
       </c>
     </row>
@@ -17693,22 +18241,22 @@
       <c r="A6">
         <v>400</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0.23724999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>0.20399999999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0.22750000000000001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0.22825000000000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>0.22775000000000001</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>0.2235</v>
       </c>
     </row>
@@ -17716,22 +18264,22 @@
       <c r="A7">
         <v>500</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.19059999999999999</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.16120000000000001</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0.18160000000000001</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>0.18340000000000001</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>0.1804</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>0.17599999999999999</v>
       </c>
     </row>
@@ -17764,22 +18312,22 @@
       <c r="A10">
         <v>100</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.63</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>0.495</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>0.56399999999999995</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>0.59499999999999997</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>0.59599999999999997</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>0.55400000000000005</v>
       </c>
     </row>
@@ -17787,22 +18335,22 @@
       <c r="A11">
         <v>200</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.3095</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>0.25950000000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>0.29399999999999998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>0.30249999999999999</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>0.29799999999999999</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>0.28799999999999998</v>
       </c>
     </row>
@@ -17810,22 +18358,22 @@
       <c r="A12">
         <v>300</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.20333333333299999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>0.17033333333299999</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>0.198666666667</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>0.20100000000000001</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>0.19633333333299999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>0.19</v>
       </c>
     </row>
@@ -17833,22 +18381,22 @@
       <c r="A13">
         <v>400</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.15225</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>0.126</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>0.14774999999999999</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>0.15125</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>0.14774999999999999</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>0.14699999999999999</v>
       </c>
     </row>
@@ -17856,22 +18404,22 @@
       <c r="A14">
         <v>500</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.12379999999999999</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>9.9199999999999997E-2</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>0.1182</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>0.1198</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>0.1168</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>0.1172</v>
       </c>
     </row>
@@ -17904,22 +18452,22 @@
       <c r="A17">
         <v>100</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.46</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>0.36799999999999999</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>0.40500000000000003</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>0.42799999999999999</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>0.42499999999999999</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>0.39500000000000002</v>
       </c>
     </row>
@@ -17927,22 +18475,22 @@
       <c r="A18">
         <v>200</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0.22450000000000001</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>0.189</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0.215</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>0.217</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>0.21249999999999999</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>0.20849999999999999</v>
       </c>
     </row>
@@ -17950,22 +18498,22 @@
       <c r="A19">
         <v>300</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.153</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>0.128</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>0.14133333333299999</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>0.14699999999999999</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>0.14033333333299999</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>0.14066666666700001</v>
       </c>
     </row>
@@ -17973,22 +18521,22 @@
       <c r="A20">
         <v>400</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.1125</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>9.4750000000000001E-2</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0.1075</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>0.11175</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>0.1075</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>0.10875</v>
       </c>
     </row>
@@ -17996,22 +18544,22 @@
       <c r="A21">
         <v>500</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>8.9599999999999999E-2</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>7.46E-2</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>8.6599999999999996E-2</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>8.8400000000000006E-2</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>8.4199999999999997E-2</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>8.6800000000000002E-2</v>
       </c>
     </row>
@@ -18044,22 +18592,22 @@
       <c r="A24">
         <v>100</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.36499999999999999</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>0.28499999999999998</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>0.29599999999999999</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>0.33100000000000002</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>0.32600000000000001</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>0.32400000000000001</v>
       </c>
     </row>
@@ -18067,22 +18615,22 @@
       <c r="A25">
         <v>200</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>0.186</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>0.14749999999999999</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>0.158</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>0.16750000000000001</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>0.17</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>0.16750000000000001</v>
       </c>
     </row>
@@ -18090,22 +18638,22 @@
       <c r="A26">
         <v>300</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>0.119666666667</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>9.9333333333299995E-2</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>0.10199999999999999</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>0.112333333333</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>0.112333333333</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>0.113</v>
       </c>
     </row>
@@ -18113,22 +18661,22 @@
       <c r="A27">
         <v>400</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>8.9749999999999996E-2</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>7.4499999999999997E-2</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>7.775E-2</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>8.4750000000000006E-2</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>8.3250000000000005E-2</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>8.6249999999999993E-2</v>
       </c>
     </row>
@@ -18136,22 +18684,22 @@
       <c r="A28">
         <v>500</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>7.3200000000000001E-2</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>5.9799999999999999E-2</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>6.6400000000000001E-2</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>6.7599999999999993E-2</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>6.9199999999999998E-2</v>
       </c>
     </row>
@@ -18162,7 +18710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -18738,7 +19286,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>